<commit_message>
update dataset final revisions
</commit_message>
<xml_diff>
--- a/data/species_lists/Land- en freshwater molluscs Gran Canaria.xlsx
+++ b/data/species_lists/Land- en freshwater molluscs Gran Canaria.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WARD\OneDrive - UGent\School\1ste master\sem_2\Project\data\species_lists\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WARD\OneDrive - UGent\School\1ste master\sem_2\Project\landsnails-occurrences\data\species_lists\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="180" documentId="13_ncr:1_{C9372428-8ECE-4D62-B5B2-9E20A3A75ACC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{179768EC-7E66-43D3-AB63-2F72A9B1DE08}"/>
+  <xr:revisionPtr revIDLastSave="180" documentId="13_ncr:1_{C9372428-8ECE-4D62-B5B2-9E20A3A75ACC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{179768EC-7E66-43D3-AB63-2F72A9B1DE08}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1440,8 +1440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D69" zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
-      <selection activeCell="H88" sqref="H88"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G74" sqref="G74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3606,9 +3606,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE596B77-0852-4209-8697-1232F4F8C9A3}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>

</xml_diff>